<commit_message>
Revert "refactor: 엑셀 데이터 추가"
</commit_message>
<xml_diff>
--- a/restaurants.xlsx
+++ b/restaurants.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
   <si>
     <t>Category</t>
   </si>
@@ -165,293 +165,13 @@
   </si>
   <si>
     <t>https://naver.me/GjGp3jga</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9.6"/>
-        <color rgb="FF0D0D0D"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>육육면관</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://naver.me/FBJzms4k</t>
-  </si>
-  <si>
-    <t>japanese</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>스시노칸도</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://naver.me/GcjTyVX1</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9.6"/>
-        <color rgb="FF0D0D0D"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>가츠시</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://naver.me/5rZm4xea</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9.6"/>
-        <color rgb="FF0D0D0D"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>개미집</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://naver.me/GLKAR7va</t>
-  </si>
-  <si>
-    <t>korean</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9.6"/>
-        <color rgb="FF0D0D0D"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>알촌</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://naver.me/xevcrAc4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>fastfood</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9.6"/>
-        <color rgb="FF0D0D0D"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>맥도날드</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://naver.me/x9JB8DQv</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9.6"/>
-        <color rgb="FF0D0D0D"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>서브웨이</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://naver.me/xL1sPTMl</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>kfc</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://naver.me/5U1zULFV</t>
-  </si>
-  <si>
-    <t>https://naver.me/xRQbtClM</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9.6"/>
-        <color rgb="FF0D0D0D"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>왕돈까</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.6"/>
-        <color rgb="FF0D0D0D"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-      </rPr>
-      <t>&amp;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.6"/>
-        <color rgb="FF0D0D0D"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>왕냉면</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9.6"/>
-        <color rgb="FF0D0D0D"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>춘리마라탕</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://naver.me/5Qu5hL57</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9.6"/>
-        <color rgb="FF0D0D0D"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>마라입구</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://naver.me/GYTyrLky</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://naver.me/GkKqCRFQ</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9.6"/>
-        <color rgb="FF0D0D0D"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>고을칼국수</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://naver.me/Gvkc1Xex</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9.6"/>
-        <color rgb="FF0D0D0D"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>사대분식</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://naver.me/FDQn4Aya</t>
-  </si>
-  <si>
-    <t>혼다라멘</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9.6"/>
-        <color rgb="FF0D0D0D"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>은혜즉석떡볶이</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://naver.me/F9QpQPR9</t>
-  </si>
-  <si>
-    <t>https://naver.me/F1Iswiju</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9.6"/>
-        <color rgb="FF0D0D0D"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>세종김밥떡볶이</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>https://naver.me/IgThe734</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9.6"/>
-        <color rgb="FF0D0D0D"/>
-        <rFont val="맑은 고딕"/>
-        <family val="2"/>
-        <charset val="129"/>
-      </rPr>
-      <t>얌샘김밥</t>
-    </r>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -488,13 +208,6 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9.6"/>
-      <color rgb="FF0D0D0D"/>
-      <name val="맑은 고딕"/>
-      <family val="2"/>
-      <charset val="129"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -510,7 +223,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -568,15 +281,6 @@
       <bottom style="medium">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -588,7 +292,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -602,21 +306,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -900,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1144,201 +833,14 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="7" t="s">
-        <v>49</v>
+      <c r="A22" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>45</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>38</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>38</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C29" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="C30" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C34" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C35" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C36" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B37" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B38" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="C38" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B39" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1365,24 +867,8 @@
     <hyperlink ref="C20" r:id="rId19"/>
     <hyperlink ref="C21" r:id="rId20"/>
     <hyperlink ref="C22" r:id="rId21"/>
-    <hyperlink ref="C23" r:id="rId22"/>
-    <hyperlink ref="C24" r:id="rId23"/>
-    <hyperlink ref="C25" r:id="rId24"/>
-    <hyperlink ref="C26" r:id="rId25"/>
-    <hyperlink ref="C27" r:id="rId26"/>
-    <hyperlink ref="C28" r:id="rId27"/>
-    <hyperlink ref="C29" r:id="rId28"/>
-    <hyperlink ref="C30" r:id="rId29"/>
-    <hyperlink ref="C31" r:id="rId30"/>
-    <hyperlink ref="C32" r:id="rId31"/>
-    <hyperlink ref="C33" r:id="rId32"/>
-    <hyperlink ref="C34" r:id="rId33"/>
-    <hyperlink ref="C35" r:id="rId34"/>
-    <hyperlink ref="C37" r:id="rId35"/>
-    <hyperlink ref="C38" r:id="rId36"/>
-    <hyperlink ref="C39" r:id="rId37"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId38"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feature:Modify HTML UI final
</commit_message>
<xml_diff>
--- a/restaurants.xlsx
+++ b/restaurants.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\student\Desktop\김성헌\VSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\student\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="100">
   <si>
     <t>Category</t>
   </si>
@@ -165,13 +165,392 @@
   </si>
   <si>
     <t>https://naver.me/GjGp3jga</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>육육면관</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://naver.me/FBJzms4k</t>
+  </si>
+  <si>
+    <t>japanese</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>스시노칸도</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://naver.me/GcjTyVX1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>가츠시</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://naver.me/5rZm4xea</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>개미집</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://naver.me/GLKAR7va</t>
+  </si>
+  <si>
+    <t>korean</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>알촌</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://naver.me/xevcrAc4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fastfood</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>맥도날드</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://naver.me/x9JB8DQv</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>서브웨이</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://naver.me/xL1sPTMl</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>kfc</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://naver.me/5U1zULFV</t>
+  </si>
+  <si>
+    <t>https://naver.me/xRQbtClM</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>왕돈까</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="Segoe UI"/>
+        <family val="2"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>왕냉면</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>춘리마라탕</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://naver.me/5Qu5hL57</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>마라입구</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://naver.me/GYTyrLky</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://naver.me/GkKqCRFQ</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>고을칼국수</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://naver.me/Gvkc1Xex</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>사대분식</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://naver.me/FDQn4Aya</t>
+  </si>
+  <si>
+    <t>혼다라멘</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>은혜즉석떡볶이</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://naver.me/F9QpQPR9</t>
+  </si>
+  <si>
+    <t>https://naver.me/F1Iswiju</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>세종김밥떡볶이</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://naver.me/IgThe734</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>얌샘김밥</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>alcohol</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>alcohol</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>쿠시노아</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://naver.me/xech8kTf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시멘트서울</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://naver.me/GrqEjtKA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://naver.me/xyjIgqFf</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>무이</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>아도겐</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://naver.me/xEqmvCdW</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>그냥포차</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://naver.me/xL15Xw0z</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>서울포차</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://naver.me/5lZCrrU3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>포시즌버거</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://naver.me/5yBPiPWo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,6 +587,26 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9.6"/>
+      <color rgb="FF0D0D0D"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222225"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.6"/>
+      <color rgb="FF0D0D0D"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -223,7 +622,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -283,6 +682,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -292,7 +700,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -306,6 +714,30 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -589,10 +1021,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -833,14 +1265,278 @@
       </c>
     </row>
     <row r="22" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="3" t="s">
-        <v>38</v>
+      <c r="A22" s="7" t="s">
+        <v>49</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>45</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C36" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -867,8 +1563,31 @@
     <hyperlink ref="C20" r:id="rId19"/>
     <hyperlink ref="C21" r:id="rId20"/>
     <hyperlink ref="C22" r:id="rId21"/>
+    <hyperlink ref="C23" r:id="rId22"/>
+    <hyperlink ref="C24" r:id="rId23"/>
+    <hyperlink ref="C25" r:id="rId24"/>
+    <hyperlink ref="C26" r:id="rId25"/>
+    <hyperlink ref="C27" r:id="rId26"/>
+    <hyperlink ref="C28" r:id="rId27"/>
+    <hyperlink ref="C29" r:id="rId28"/>
+    <hyperlink ref="C30" r:id="rId29"/>
+    <hyperlink ref="C31" r:id="rId30"/>
+    <hyperlink ref="C32" r:id="rId31"/>
+    <hyperlink ref="C33" r:id="rId32"/>
+    <hyperlink ref="C34" r:id="rId33"/>
+    <hyperlink ref="C35" r:id="rId34"/>
+    <hyperlink ref="C37" r:id="rId35"/>
+    <hyperlink ref="C38" r:id="rId36"/>
+    <hyperlink ref="C39" r:id="rId37"/>
+    <hyperlink ref="C40" r:id="rId38"/>
+    <hyperlink ref="C41" r:id="rId39"/>
+    <hyperlink ref="C42" r:id="rId40"/>
+    <hyperlink ref="C43" r:id="rId41"/>
+    <hyperlink ref="C44" r:id="rId42"/>
+    <hyperlink ref="C45" r:id="rId43"/>
+    <hyperlink ref="C46" r:id="rId44"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId22"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId45"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feature:Modify HTML UI fn
</commit_message>
<xml_diff>
--- a/restaurants.xlsx
+++ b/restaurants.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\student\Desktop\김성헌\VSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\student\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="100">
   <si>
     <t>Category</t>
   </si>
@@ -444,6 +444,105 @@
       </rPr>
       <t>얌샘김밥</t>
     </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>alcohol</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>alcohol</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>쿠시노아</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://naver.me/xech8kTf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>시멘트서울</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://naver.me/GrqEjtKA</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://naver.me/xyjIgqFf</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>무이</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>아도겐</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://naver.me/xEqmvCdW</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>그냥포차</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://naver.me/xL15Xw0z</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9.6"/>
+        <color rgb="FF0D0D0D"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+        <charset val="129"/>
+      </rPr>
+      <t>서울포차</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://naver.me/5lZCrrU3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>포시즌버거</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://naver.me/5yBPiPWo</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -451,7 +550,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -493,6 +592,19 @@
       <color rgb="FF0D0D0D"/>
       <name val="맑은 고딕"/>
       <family val="2"/>
+      <charset val="129"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF222225"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9.6"/>
+      <color rgb="FF0D0D0D"/>
+      <name val="돋움"/>
+      <family val="3"/>
       <charset val="129"/>
     </font>
   </fonts>
@@ -588,7 +700,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -617,6 +729,15 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -900,10 +1021,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C39"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1339,6 +1460,83 @@
       </c>
       <c r="C39" s="6" t="s">
         <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C45" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A46" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1381,8 +1579,15 @@
     <hyperlink ref="C37" r:id="rId35"/>
     <hyperlink ref="C38" r:id="rId36"/>
     <hyperlink ref="C39" r:id="rId37"/>
+    <hyperlink ref="C40" r:id="rId38"/>
+    <hyperlink ref="C41" r:id="rId39"/>
+    <hyperlink ref="C42" r:id="rId40"/>
+    <hyperlink ref="C43" r:id="rId41"/>
+    <hyperlink ref="C44" r:id="rId42"/>
+    <hyperlink ref="C45" r:id="rId43"/>
+    <hyperlink ref="C46" r:id="rId44"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId38"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId45"/>
 </worksheet>
 </file>
</xml_diff>